<commit_message>
t7b - com incertezas
</commit_message>
<xml_diff>
--- a/T7B - PONTES.xlsx
+++ b/T7B - PONTES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunop\OneDrive\Documentos\GitHub\LABSFISICAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ECAA440-097B-40C8-8209-8440850F3CEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2CB3210-C327-4371-95E4-309CAF0F19AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{5612D8A9-4F74-4819-A33D-9867F612D722}"/>
   </bookViews>
@@ -271,6 +271,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -314,7 +317,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -324,6 +327,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -381,7 +390,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -401,6 +410,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -416,7 +428,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -548,7 +566,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="3"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
@@ -741,7 +759,7 @@
             <c:numRef>
               <c:f>'Parte 2'!$C$2:$C$52</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="51"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -921,7 +939,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="3"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
@@ -1100,7 +1118,7 @@
             <c:numRef>
               <c:f>'Parte 2'!$I$2:$I$52</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="51"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -1280,7 +1298,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="3"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
@@ -1459,7 +1477,7 @@
             <c:numRef>
               <c:f>'Parte 2'!$J$2:$J$52</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="51"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -1852,7 +1870,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4254,7 +4272,7 @@
   <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4328,7 +4346,7 @@
         <f>ABS(F2-C2)/C2</f>
         <v>5.1969823973177249E-3</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="7" t="s">
         <v>42</v>
       </c>
       <c r="L2" s="3" t="s">
@@ -4337,7 +4355,7 @@
       <c r="M2" s="1">
         <v>1000</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="8" t="s">
         <v>40</v>
       </c>
       <c r="O2" s="3" t="s">
@@ -4378,7 +4396,7 @@
         <f t="shared" ref="I3:I6" si="4">ABS(F3-C3)/C3</f>
         <v>2.0896226415094424E-2</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="7" t="s">
         <v>43</v>
       </c>
       <c r="L3" s="3" t="s">
@@ -4387,7 +4405,7 @@
       <c r="M3" s="1">
         <v>1000</v>
       </c>
-      <c r="N3" s="8"/>
+      <c r="N3" s="9"/>
       <c r="O3" s="3" t="s">
         <v>17</v>
       </c>
@@ -4426,7 +4444,7 @@
         <f t="shared" si="4"/>
         <v>1.518518518518513E-2</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="7" t="s">
         <v>44</v>
       </c>
     </row>
@@ -4434,7 +4452,7 @@
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="15" t="s">
         <v>39</v>
       </c>
       <c r="C5" s="1">
@@ -4463,7 +4481,7 @@
         <f t="shared" si="4"/>
         <v>1.1155015197568334E-2</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="7" t="s">
         <v>45</v>
       </c>
     </row>
@@ -4471,7 +4489,7 @@
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="15" t="s">
         <v>39</v>
       </c>
       <c r="C6" s="1">
@@ -4500,7 +4518,7 @@
         <f t="shared" si="4"/>
         <v>4.5016077170417276E-3</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="J6" s="7" t="s">
         <v>46</v>
       </c>
     </row>
@@ -4522,8 +4540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2744CCB0-2F7D-4947-8B22-CBAF80B9ABCC}">
   <dimension ref="A1:R52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4577,11 +4595,13 @@
       <c r="B2" s="1">
         <v>0</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="13">
         <f>B2*0.001</f>
         <v>0</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E2" s="1">
         <v>1.0920000000000001</v>
       </c>
@@ -4593,16 +4613,18 @@
         <f>F2-$F$2</f>
         <v>0</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1">
+      <c r="H2" s="1">
+        <v>24</v>
+      </c>
+      <c r="I2" s="13">
         <f>(G2*$P$2)/(4*$P$3+2*G2)</f>
         <v>0</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="13">
         <f>(G2*$P$2)/(4*$P$3)</f>
         <v>0</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K2" s="13">
         <f>G2*$O$24+$P$24</f>
         <v>1.9621666224476156E-4</v>
       </c>
@@ -4624,11 +4646,13 @@
       <c r="B3" s="1">
         <v>0.23499999999999999</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="13">
         <f t="shared" ref="C3:C52" si="0">B3*0.001</f>
         <v>2.3499999999999999E-4</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E3" s="1">
         <v>1.093</v>
       </c>
@@ -4640,16 +4664,18 @@
         <f t="shared" ref="G3:G52" si="2">F3-$F$2</f>
         <v>1</v>
       </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1">
+      <c r="H3" s="1">
+        <v>24</v>
+      </c>
+      <c r="I3" s="13">
         <f t="shared" ref="I3:I52" si="3">(G3*$P$2)/(4*$P$3+2*G3)</f>
         <v>1.060758797653959E-4</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3" s="13">
         <f t="shared" ref="J3:J52" si="4">(G3*$P$2)/(4*$P$3)</f>
         <v>1.0612450719721279E-4</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3" s="13">
         <f t="shared" ref="K3:K52" si="5">G3*$O$24+$P$24</f>
         <v>3.023803534802076E-4</v>
       </c>
@@ -4671,11 +4697,13 @@
       <c r="B4" s="1">
         <v>0.47499999999999998</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="13">
         <f t="shared" si="0"/>
         <v>4.75E-4</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E4" s="1">
         <v>1.0940000000000001</v>
       </c>
@@ -4687,16 +4715,18 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1">
+      <c r="H4" s="1">
+        <v>24</v>
+      </c>
+      <c r="I4" s="13">
         <f t="shared" si="3"/>
         <v>2.1205459375286251E-4</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4" s="13">
         <f t="shared" si="4"/>
         <v>2.1224901439442559E-4</v>
       </c>
-      <c r="K4" s="1">
+      <c r="K4" s="13">
         <f t="shared" si="5"/>
         <v>4.0854404471565365E-4</v>
       </c>
@@ -4712,11 +4742,13 @@
       <c r="B5" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="13">
         <f t="shared" si="0"/>
         <v>5.6000000000000006E-4</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E5" s="1">
         <v>1.095</v>
       </c>
@@ -4728,16 +4760,18 @@
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1">
+      <c r="H5" s="1">
+        <v>25</v>
+      </c>
+      <c r="I5" s="13">
         <f t="shared" si="3"/>
         <v>3.1793627540743454E-4</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5" s="13">
         <f t="shared" si="4"/>
         <v>3.1837352159163837E-4</v>
       </c>
-      <c r="K5" s="1">
+      <c r="K5" s="13">
         <f>G5*$O$24+$P$24</f>
         <v>5.1470773595109964E-4</v>
       </c>
@@ -4753,11 +4787,13 @@
       <c r="B6" s="1">
         <v>0.64</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="13">
         <f t="shared" si="0"/>
         <v>6.4000000000000005E-4</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E6" s="1">
         <v>1.0960000000000001</v>
       </c>
@@ -4769,16 +4805,18 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1">
+      <c r="H6" s="1">
+        <v>25</v>
+      </c>
+      <c r="I6" s="13">
         <f t="shared" si="3"/>
         <v>4.237210579298984E-4</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="13">
         <f t="shared" si="4"/>
         <v>4.2449802878885117E-4</v>
       </c>
-      <c r="K6" s="1">
+      <c r="K6" s="13">
         <f t="shared" si="5"/>
         <v>6.2087142718654574E-4</v>
       </c>
@@ -4794,11 +4832,13 @@
       <c r="B7" s="1">
         <v>0.72699999999999998</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="13">
         <f t="shared" si="0"/>
         <v>7.27E-4</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="D7" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E7" s="1">
         <v>1.097</v>
       </c>
@@ -4810,16 +4850,18 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1">
+      <c r="H7" s="1">
+        <v>25</v>
+      </c>
+      <c r="I7" s="13">
         <f t="shared" si="3"/>
         <v>5.2940907427735087E-4</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="13">
         <f t="shared" si="4"/>
         <v>5.3062253598606393E-4</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7" s="13">
         <f t="shared" si="5"/>
         <v>7.2703511842199184E-4</v>
       </c>
@@ -4835,11 +4877,13 @@
       <c r="B8" s="1">
         <v>0.81</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="13">
         <f t="shared" si="0"/>
         <v>8.1000000000000006E-4</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E8" s="1">
         <v>1.0980000000000001</v>
       </c>
@@ -4851,16 +4895,18 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1">
+      <c r="H8" s="1">
+        <v>25</v>
+      </c>
+      <c r="I8" s="13">
         <f t="shared" si="3"/>
         <v>6.35000457163756E-4</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8" s="13">
         <f t="shared" si="4"/>
         <v>6.3674704318327673E-4</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K8" s="13">
         <f t="shared" si="5"/>
         <v>8.3319880965743783E-4</v>
       </c>
@@ -4876,11 +4922,13 @@
       <c r="B9" s="1">
         <v>0.89300000000000002</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="13">
         <f t="shared" si="0"/>
         <v>8.9300000000000002E-4</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E9" s="1">
         <v>1.0980000000000001</v>
       </c>
@@ -4892,16 +4940,18 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1">
+      <c r="H9" s="1">
+        <v>25</v>
+      </c>
+      <c r="I9" s="13">
         <f t="shared" si="3"/>
         <v>6.35000457163756E-4</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="13">
         <f t="shared" si="4"/>
         <v>6.3674704318327673E-4</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K9" s="13">
         <f t="shared" si="5"/>
         <v>8.3319880965743783E-4</v>
       </c>
@@ -4917,11 +4967,13 @@
       <c r="B10" s="1">
         <v>0.97399999999999998</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="13">
         <f t="shared" si="0"/>
         <v>9.7400000000000004E-4</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="D10" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E10" s="1">
         <v>1.099</v>
       </c>
@@ -4933,16 +4985,18 @@
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1">
+      <c r="H10" s="1">
+        <v>26</v>
+      </c>
+      <c r="I10" s="13">
         <f t="shared" si="3"/>
         <v>7.4049533906050079E-4</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10" s="13">
         <f t="shared" si="4"/>
         <v>7.4287155038048954E-4</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K10" s="13">
         <f t="shared" si="5"/>
         <v>9.3936250089288382E-4</v>
       </c>
@@ -4958,11 +5012,13 @@
       <c r="B11" s="1">
         <v>1.0620000000000001</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="13">
         <f t="shared" si="0"/>
         <v>1.062E-3</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E11" s="1">
         <v>1.1000000000000001</v>
       </c>
@@ -4974,16 +5030,18 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1">
+      <c r="H11" s="1">
+        <v>26</v>
+      </c>
+      <c r="I11" s="13">
         <f t="shared" si="3"/>
         <v>8.4589385219694898E-4</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J11" s="13">
         <f t="shared" si="4"/>
         <v>8.4899605757770235E-4</v>
       </c>
-      <c r="K11" s="1">
+      <c r="K11" s="13">
         <f t="shared" si="5"/>
         <v>1.0455261921283299E-3</v>
       </c>
@@ -4999,11 +5057,13 @@
       <c r="B12" s="1">
         <v>1.1319999999999999</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="13">
         <f t="shared" si="0"/>
         <v>1.132E-3</v>
       </c>
-      <c r="D12" s="1"/>
+      <c r="D12" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E12" s="1">
         <v>1.101</v>
       </c>
@@ -5015,16 +5075,18 @@
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1">
+      <c r="H12" s="1">
+        <v>26</v>
+      </c>
+      <c r="I12" s="13">
         <f t="shared" si="3"/>
         <v>9.511961285609933E-4</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J12" s="13">
         <f t="shared" si="4"/>
         <v>9.5512056477491515E-4</v>
       </c>
-      <c r="K12" s="1">
+      <c r="K12" s="13">
         <f t="shared" si="5"/>
         <v>1.151689883363776E-3</v>
       </c>
@@ -5040,11 +5102,13 @@
       <c r="B13" s="1">
         <v>1.2350000000000001</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="13">
         <f t="shared" si="0"/>
         <v>1.2350000000000002E-3</v>
       </c>
-      <c r="D13" s="1"/>
+      <c r="D13" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E13" s="1">
         <v>1.101</v>
       </c>
@@ -5056,16 +5120,18 @@
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1">
+      <c r="H13" s="1">
+        <v>26</v>
+      </c>
+      <c r="I13" s="13">
         <f t="shared" si="3"/>
         <v>9.511961285609933E-4</v>
       </c>
-      <c r="J13" s="1">
+      <c r="J13" s="13">
         <f t="shared" si="4"/>
         <v>9.5512056477491515E-4</v>
       </c>
-      <c r="K13" s="1">
+      <c r="K13" s="13">
         <f t="shared" si="5"/>
         <v>1.151689883363776E-3</v>
       </c>
@@ -5081,11 +5147,13 @@
       <c r="B14" s="1">
         <v>1.3</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="13">
         <f t="shared" si="0"/>
         <v>1.3000000000000002E-3</v>
       </c>
-      <c r="D14" s="1"/>
+      <c r="D14" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E14" s="1">
         <v>1.1020000000000001</v>
       </c>
@@ -5097,16 +5165,18 @@
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1">
+      <c r="H14" s="1">
+        <v>26</v>
+      </c>
+      <c r="I14" s="13">
         <f t="shared" si="3"/>
         <v>1.0564022998996074E-3</v>
       </c>
-      <c r="J14" s="1">
+      <c r="J14" s="13">
         <f t="shared" si="4"/>
         <v>1.0612450719721279E-3</v>
       </c>
-      <c r="K14" s="1">
+      <c r="K14" s="13">
         <f t="shared" si="5"/>
         <v>1.2578535745992221E-3</v>
       </c>
@@ -5122,11 +5192,13 @@
       <c r="B15" s="1">
         <v>1.379</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="13">
         <f t="shared" si="0"/>
         <v>1.379E-3</v>
       </c>
-      <c r="D15" s="1"/>
+      <c r="D15" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E15" s="1">
         <v>1.103</v>
       </c>
@@ -5138,16 +5210,18 @@
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1">
+      <c r="H15" s="1">
+        <v>27</v>
+      </c>
+      <c r="I15" s="13">
         <f t="shared" si="3"/>
         <v>1.1615124977193943E-3</v>
       </c>
-      <c r="J15" s="1">
+      <c r="J15" s="13">
         <f t="shared" si="4"/>
         <v>1.1673695791693407E-3</v>
       </c>
-      <c r="K15" s="1">
+      <c r="K15" s="13">
         <f t="shared" si="5"/>
         <v>1.364017265834668E-3</v>
       </c>
@@ -5163,11 +5237,13 @@
       <c r="B16" s="1">
         <v>1.46</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="13">
         <f t="shared" si="0"/>
         <v>1.4599999999999999E-3</v>
       </c>
-      <c r="D16" s="1"/>
+      <c r="D16" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E16" s="1">
         <v>1.1040000000000001</v>
       </c>
@@ -5179,16 +5255,18 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1">
+      <c r="H16" s="1">
+        <v>27</v>
+      </c>
+      <c r="I16" s="13">
         <f t="shared" si="3"/>
         <v>1.2665268532871341E-3</v>
       </c>
-      <c r="J16" s="1">
+      <c r="J16" s="13">
         <f t="shared" si="4"/>
         <v>1.2734940863665535E-3</v>
       </c>
-      <c r="K16" s="1">
+      <c r="K16" s="13">
         <f t="shared" si="5"/>
         <v>1.4701809570701141E-3</v>
       </c>
@@ -5204,11 +5282,13 @@
       <c r="B17" s="1">
         <v>1.5369999999999999</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="13">
         <f t="shared" si="0"/>
         <v>1.537E-3</v>
       </c>
-      <c r="D17" s="1"/>
+      <c r="D17" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E17" s="1">
         <v>1.105</v>
       </c>
@@ -5220,16 +5300,18 @@
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1">
+      <c r="H17" s="1">
+        <v>27</v>
+      </c>
+      <c r="I17" s="13">
         <f t="shared" si="3"/>
         <v>1.3714454976303317E-3</v>
       </c>
-      <c r="J17" s="1">
+      <c r="J17" s="13">
         <f t="shared" si="4"/>
         <v>1.3796185935637663E-3</v>
       </c>
-      <c r="K17" s="1">
+      <c r="K17" s="13">
         <f t="shared" si="5"/>
         <v>1.5763446483055602E-3</v>
       </c>
@@ -5245,11 +5327,13 @@
       <c r="B18" s="1">
         <v>1.61</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="13">
         <f t="shared" si="0"/>
         <v>1.6100000000000001E-3</v>
       </c>
-      <c r="D18" s="1"/>
+      <c r="D18" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E18" s="1">
         <v>1.105</v>
       </c>
@@ -5261,16 +5345,18 @@
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1">
+      <c r="H18" s="1">
+        <v>27</v>
+      </c>
+      <c r="I18" s="13">
         <f t="shared" si="3"/>
         <v>1.3714454976303317E-3</v>
       </c>
-      <c r="J18" s="1">
+      <c r="J18" s="13">
         <f t="shared" si="4"/>
         <v>1.3796185935637663E-3</v>
       </c>
-      <c r="K18" s="1">
+      <c r="K18" s="13">
         <f t="shared" si="5"/>
         <v>1.5763446483055602E-3</v>
       </c>
@@ -5286,11 +5372,13 @@
       <c r="B19" s="1">
         <v>1.6919999999999999</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="13">
         <f t="shared" si="0"/>
         <v>1.6919999999999999E-3</v>
       </c>
-      <c r="D19" s="1"/>
+      <c r="D19" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E19" s="1">
         <v>1.1060000000000001</v>
       </c>
@@ -5302,16 +5390,18 @@
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1">
+      <c r="H19" s="1">
+        <v>27</v>
+      </c>
+      <c r="I19" s="13">
         <f t="shared" si="3"/>
         <v>1.4762685615377607E-3</v>
       </c>
-      <c r="J19" s="1">
+      <c r="J19" s="13">
         <f t="shared" si="4"/>
         <v>1.4857431007609791E-3</v>
       </c>
-      <c r="K19" s="1">
+      <c r="K19" s="13">
         <f t="shared" si="5"/>
         <v>1.6825083395410061E-3</v>
       </c>
@@ -5327,11 +5417,13 @@
       <c r="B20" s="1">
         <v>1.67</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="13">
         <f t="shared" si="0"/>
         <v>1.67E-3</v>
       </c>
-      <c r="D20" s="1"/>
+      <c r="D20" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E20" s="1">
         <v>1.107</v>
       </c>
@@ -5343,16 +5435,18 @@
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1">
+      <c r="H20" s="1">
+        <v>28</v>
+      </c>
+      <c r="I20" s="13">
         <f t="shared" si="3"/>
         <v>1.5809961755600074E-3</v>
       </c>
-      <c r="J20" s="1">
+      <c r="J20" s="13">
         <f t="shared" si="4"/>
         <v>1.5918676079581919E-3</v>
       </c>
-      <c r="K20" s="1">
+      <c r="K20" s="13">
         <f t="shared" si="5"/>
         <v>1.7886720307764522E-3</v>
       </c>
@@ -5368,11 +5462,13 @@
       <c r="B21" s="1">
         <v>1.843</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="13">
         <f t="shared" si="0"/>
         <v>1.843E-3</v>
       </c>
-      <c r="D21" s="1"/>
+      <c r="D21" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E21" s="1">
         <v>1.107</v>
       </c>
@@ -5384,16 +5480,18 @@
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1">
+      <c r="H21" s="1">
+        <v>28</v>
+      </c>
+      <c r="I21" s="13">
         <f t="shared" si="3"/>
         <v>1.5809961755600074E-3</v>
       </c>
-      <c r="J21" s="1">
+      <c r="J21" s="13">
         <f t="shared" si="4"/>
         <v>1.5918676079581919E-3</v>
       </c>
-      <c r="K21" s="1">
+      <c r="K21" s="13">
         <f t="shared" si="5"/>
         <v>1.7886720307764522E-3</v>
       </c>
@@ -5409,11 +5507,13 @@
       <c r="B22" s="1">
         <v>1.925</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="13">
         <f t="shared" si="0"/>
         <v>1.9250000000000001E-3</v>
       </c>
-      <c r="D22" s="1"/>
+      <c r="D22" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E22" s="1">
         <v>1.1080000000000001</v>
       </c>
@@ -5425,16 +5525,18 @@
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1">
+      <c r="H22" s="1">
+        <v>28</v>
+      </c>
+      <c r="I22" s="13">
         <f t="shared" si="3"/>
         <v>1.6856284700100118E-3</v>
       </c>
-      <c r="J22" s="1">
+      <c r="J22" s="13">
         <f t="shared" si="4"/>
         <v>1.6979921151554047E-3</v>
       </c>
-      <c r="K22" s="1">
+      <c r="K22" s="13">
         <f t="shared" si="5"/>
         <v>1.8948357220118983E-3</v>
       </c>
@@ -5450,11 +5552,13 @@
       <c r="B23" s="1">
         <v>2</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="13">
         <f t="shared" si="0"/>
         <v>2E-3</v>
       </c>
-      <c r="D23" s="1"/>
+      <c r="D23" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E23" s="1">
         <v>1.109</v>
       </c>
@@ -5466,16 +5570,18 @@
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1">
+      <c r="H23" s="1">
+        <v>28</v>
+      </c>
+      <c r="I23" s="13">
         <f t="shared" si="3"/>
         <v>1.79016557496361E-3</v>
       </c>
-      <c r="J23" s="1">
+      <c r="J23" s="13">
         <f t="shared" si="4"/>
         <v>1.8041166223526177E-3</v>
       </c>
-      <c r="K23" s="1">
+      <c r="K23" s="13">
         <f t="shared" si="5"/>
         <v>2.0009994132473442E-3</v>
       </c>
@@ -5483,13 +5589,13 @@
         <f t="shared" si="6"/>
         <v>-9.9941324734412196E-7</v>
       </c>
-      <c r="N23" s="9" t="s">
+      <c r="N23" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="O23" s="9"/>
-      <c r="P23" s="9"/>
-      <c r="Q23" s="9"/>
-      <c r="R23" s="9"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
@@ -5498,12 +5604,14 @@
       <c r="B24" s="1">
         <v>2.0720000000000001</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="13">
         <f t="shared" si="0"/>
         <v>2.0720000000000001E-3</v>
       </c>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1">
+      <c r="D24" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="E24" s="14">
         <v>1.1100000000000001</v>
       </c>
       <c r="F24" s="1">
@@ -5514,16 +5622,18 @@
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1">
+      <c r="H24" s="1">
+        <v>28</v>
+      </c>
+      <c r="I24" s="13">
         <f t="shared" si="3"/>
         <v>1.8946076202600707E-3</v>
       </c>
-      <c r="J24" s="1">
+      <c r="J24" s="13">
         <f t="shared" si="4"/>
         <v>1.9102411295498303E-3</v>
       </c>
-      <c r="K24" s="1">
+      <c r="K24" s="13">
         <f t="shared" si="5"/>
         <v>2.1071631044827905E-3</v>
       </c>
@@ -5541,10 +5651,10 @@
       <c r="P24" s="5">
         <v>1.9621666224476156E-4</v>
       </c>
-      <c r="Q24" s="10" t="s">
+      <c r="Q24" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="R24" s="11"/>
+      <c r="R24" s="12"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
@@ -5553,11 +5663,13 @@
       <c r="B25" s="1">
         <v>2.1760000000000002</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="13">
         <f t="shared" si="0"/>
         <v>2.1760000000000004E-3</v>
       </c>
-      <c r="D25" s="1"/>
+      <c r="D25" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E25" s="1">
         <v>1.111</v>
       </c>
@@ -5569,16 +5681,18 @@
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1">
+      <c r="H25" s="1">
+        <v>29</v>
+      </c>
+      <c r="I25" s="13">
         <f t="shared" si="3"/>
         <v>1.9989547355026361E-3</v>
       </c>
-      <c r="J25" s="1">
+      <c r="J25" s="13">
         <f t="shared" si="4"/>
         <v>2.0163656367470431E-3</v>
       </c>
-      <c r="K25" s="1">
+      <c r="K25" s="13">
         <f t="shared" si="5"/>
         <v>2.2133267957182364E-3</v>
       </c>
@@ -5595,10 +5709,10 @@
       <c r="P25" s="5">
         <v>1.3883972095916352E-5</v>
       </c>
-      <c r="Q25" s="9" t="s">
+      <c r="Q25" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="R25" s="9"/>
+      <c r="R25" s="10"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
@@ -5607,11 +5721,13 @@
       <c r="B26" s="1">
         <v>2.3039999999999998</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="13">
         <f t="shared" si="0"/>
         <v>2.3040000000000001E-3</v>
       </c>
-      <c r="D26" s="1"/>
+      <c r="D26" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E26" s="1">
         <v>1.1120000000000001</v>
       </c>
@@ -5623,16 +5739,18 @@
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1">
+      <c r="H26" s="1">
+        <v>29</v>
+      </c>
+      <c r="I26" s="13">
         <f t="shared" si="3"/>
         <v>2.103207050059053E-3</v>
       </c>
-      <c r="J26" s="1">
+      <c r="J26" s="13">
         <f t="shared" si="4"/>
         <v>2.1224901439442557E-3</v>
       </c>
-      <c r="K26" s="1">
+      <c r="K26" s="13">
         <f t="shared" si="5"/>
         <v>2.3194904869536827E-3</v>
       </c>
@@ -5649,10 +5767,10 @@
       <c r="P26" s="5">
         <v>4.9693147055673696E-5</v>
       </c>
-      <c r="Q26" s="9" t="s">
+      <c r="Q26" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="R26" s="9"/>
+      <c r="R26" s="10"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
@@ -5661,11 +5779,13 @@
       <c r="B27" s="1">
         <v>2.4319999999999999</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="13">
         <f t="shared" si="0"/>
         <v>2.4320000000000001E-3</v>
       </c>
-      <c r="D27" s="1"/>
+      <c r="D27" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E27" s="1">
         <v>1.113</v>
       </c>
@@ -5677,16 +5797,18 @@
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1">
+      <c r="H27" s="1">
+        <v>29</v>
+      </c>
+      <c r="I27" s="13">
         <f t="shared" si="3"/>
         <v>2.2073646930621141E-3</v>
       </c>
-      <c r="J27" s="1">
+      <c r="J27" s="13">
         <f t="shared" si="4"/>
         <v>2.2286146511414687E-3</v>
       </c>
-      <c r="K27" s="1">
+      <c r="K27" s="13">
         <f t="shared" si="5"/>
         <v>2.4256541781891286E-3</v>
       </c>
@@ -5702,11 +5824,13 @@
       <c r="B28" s="1">
         <v>2.5249999999999999</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="13">
         <f t="shared" si="0"/>
         <v>2.5249999999999999E-3</v>
       </c>
-      <c r="D28" s="1"/>
+      <c r="D28" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E28" s="1">
         <v>1.1140000000000001</v>
       </c>
@@ -5718,16 +5842,18 @@
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1">
+      <c r="H28" s="1">
+        <v>29</v>
+      </c>
+      <c r="I28" s="13">
         <f t="shared" si="3"/>
         <v>2.3114277934101844E-3</v>
       </c>
-      <c r="J28" s="1">
+      <c r="J28" s="13">
         <f t="shared" si="4"/>
         <v>2.3347391583386813E-3</v>
       </c>
-      <c r="K28" s="1">
+      <c r="K28" s="13">
         <f t="shared" si="5"/>
         <v>2.5318178694245744E-3</v>
       </c>
@@ -5743,11 +5869,13 @@
       <c r="B29" s="1">
         <v>2.63</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29" s="13">
         <f t="shared" si="0"/>
         <v>2.63E-3</v>
       </c>
-      <c r="D29" s="1"/>
+      <c r="D29" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E29" s="1">
         <v>1.115</v>
       </c>
@@ -5759,16 +5887,18 @@
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1">
+      <c r="H29" s="1">
+        <v>30</v>
+      </c>
+      <c r="I29" s="13">
         <f t="shared" si="3"/>
         <v>2.4153964797677375E-3</v>
       </c>
-      <c r="J29" s="1">
+      <c r="J29" s="13">
         <f t="shared" si="4"/>
         <v>2.4408636655358943E-3</v>
       </c>
-      <c r="K29" s="1">
+      <c r="K29" s="13">
         <f t="shared" si="5"/>
         <v>2.6379815606600208E-3</v>
       </c>
@@ -5784,11 +5914,13 @@
       <c r="B30" s="1">
         <v>2.7919999999999998</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="13">
         <f t="shared" si="0"/>
         <v>2.7919999999999998E-3</v>
       </c>
-      <c r="D30" s="1"/>
+      <c r="D30" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E30" s="1">
         <v>1.1160000000000001</v>
       </c>
@@ -5800,16 +5932,18 @@
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1">
+      <c r="H30" s="1">
+        <v>30</v>
+      </c>
+      <c r="I30" s="13">
         <f t="shared" si="3"/>
         <v>2.5192708805658838E-3</v>
       </c>
-      <c r="J30" s="1">
+      <c r="J30" s="13">
         <f t="shared" si="4"/>
         <v>2.5469881727331069E-3</v>
       </c>
-      <c r="K30" s="1">
+      <c r="K30" s="13">
         <f t="shared" si="5"/>
         <v>2.7441452518954666E-3</v>
       </c>
@@ -5825,11 +5959,13 @@
       <c r="B31" s="1">
         <v>2.89</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="13">
         <f t="shared" si="0"/>
         <v>2.8900000000000002E-3</v>
       </c>
-      <c r="D31" s="1"/>
+      <c r="D31" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E31" s="1">
         <v>1.117</v>
       </c>
@@ -5841,16 +5977,18 @@
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1">
+      <c r="H31" s="1">
+        <v>30</v>
+      </c>
+      <c r="I31" s="13">
         <f t="shared" si="3"/>
         <v>2.6230511240029008E-3</v>
       </c>
-      <c r="J31" s="1">
+      <c r="J31" s="13">
         <f t="shared" si="4"/>
         <v>2.65311267993032E-3</v>
       </c>
-      <c r="K31" s="1">
+      <c r="K31" s="13">
         <f t="shared" si="5"/>
         <v>2.8503089431309125E-3</v>
       </c>
@@ -5866,11 +6004,13 @@
       <c r="B32" s="1">
         <v>2.9980000000000002</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32" s="13">
         <f t="shared" si="0"/>
         <v>2.9980000000000002E-3</v>
       </c>
-      <c r="D32" s="1"/>
+      <c r="D32" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E32" s="1">
         <v>1.1180000000000001</v>
       </c>
@@ -5882,16 +6022,18 @@
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1">
+      <c r="H32" s="1">
+        <v>30</v>
+      </c>
+      <c r="I32" s="13">
         <f t="shared" si="3"/>
         <v>2.7267373380447583E-3</v>
       </c>
-      <c r="J32" s="1">
+      <c r="J32" s="13">
         <f t="shared" si="4"/>
         <v>2.7592371871275325E-3</v>
       </c>
-      <c r="K32" s="1">
+      <c r="K32" s="13">
         <f t="shared" si="5"/>
         <v>2.9564726343663588E-3</v>
       </c>
@@ -5907,11 +6049,13 @@
       <c r="B33" s="1">
         <v>3.1</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="13">
         <f t="shared" si="0"/>
         <v>3.1000000000000003E-3</v>
       </c>
-      <c r="D33" s="1"/>
+      <c r="D33" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E33" s="1">
         <v>1.119</v>
       </c>
@@ -5923,16 +6067,18 @@
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1">
+      <c r="H33" s="1">
+        <v>31</v>
+      </c>
+      <c r="I33" s="13">
         <f t="shared" si="3"/>
         <v>2.8303296504256477E-3</v>
       </c>
-      <c r="J33" s="1">
+      <c r="J33" s="13">
         <f t="shared" si="4"/>
         <v>2.8653616943247456E-3</v>
       </c>
-      <c r="K33" s="1">
+      <c r="K33" s="13">
         <f t="shared" si="5"/>
         <v>3.0626363256018047E-3</v>
       </c>
@@ -5948,11 +6094,13 @@
       <c r="B34" s="1">
         <v>3.1930000000000001</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C34" s="13">
         <f t="shared" si="0"/>
         <v>3.1930000000000001E-3</v>
       </c>
-      <c r="D34" s="1"/>
+      <c r="D34" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E34" s="1">
         <v>1.1200000000000001</v>
       </c>
@@ -5964,16 +6112,18 @@
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1">
+      <c r="H34" s="1">
+        <v>31</v>
+      </c>
+      <c r="I34" s="13">
         <f t="shared" si="3"/>
         <v>2.9338281886485016E-3</v>
       </c>
-      <c r="J34" s="1">
+      <c r="J34" s="13">
         <f t="shared" si="4"/>
         <v>2.9714862015219582E-3</v>
       </c>
-      <c r="K34" s="1">
+      <c r="K34" s="13">
         <f t="shared" si="5"/>
         <v>3.1688000168372506E-3</v>
       </c>
@@ -5989,11 +6139,13 @@
       <c r="B35" s="1">
         <v>3.28</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="13">
         <f t="shared" si="0"/>
         <v>3.2799999999999999E-3</v>
       </c>
-      <c r="D35" s="1"/>
+      <c r="D35" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E35" s="1">
         <v>1.121</v>
       </c>
@@ -6005,16 +6157,18 @@
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1">
+      <c r="H35" s="1">
+        <v>31</v>
+      </c>
+      <c r="I35" s="13">
         <f t="shared" si="3"/>
         <v>3.0372330799855233E-3</v>
       </c>
-      <c r="J35" s="1">
+      <c r="J35" s="13">
         <f t="shared" si="4"/>
         <v>3.0776107087191712E-3</v>
       </c>
-      <c r="K35" s="1">
+      <c r="K35" s="13">
         <f t="shared" si="5"/>
         <v>3.2749637080726969E-3</v>
       </c>
@@ -6030,11 +6184,13 @@
       <c r="B36" s="1">
         <v>3.387</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="13">
         <f t="shared" si="0"/>
         <v>3.3870000000000003E-3</v>
       </c>
-      <c r="D36" s="1"/>
+      <c r="D36" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E36" s="1">
         <v>1.1220000000000001</v>
       </c>
@@ -6046,16 +6202,18 @@
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1">
+      <c r="H36" s="1">
+        <v>31</v>
+      </c>
+      <c r="I36" s="13">
         <f t="shared" si="3"/>
         <v>3.1405444514787011E-3</v>
       </c>
-      <c r="J36" s="1">
+      <c r="J36" s="13">
         <f t="shared" si="4"/>
         <v>3.1837352159163838E-3</v>
       </c>
-      <c r="K36" s="1">
+      <c r="K36" s="13">
         <f t="shared" si="5"/>
         <v>3.3811273993081428E-3</v>
       </c>
@@ -6071,11 +6229,13 @@
       <c r="B37" s="1">
         <v>3.4820000000000002</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C37" s="13">
         <f t="shared" si="0"/>
         <v>3.4820000000000003E-3</v>
       </c>
-      <c r="D37" s="1"/>
+      <c r="D37" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E37" s="1">
         <v>1.123</v>
       </c>
@@ -6087,16 +6247,18 @@
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1">
+      <c r="H37" s="1">
+        <v>32</v>
+      </c>
+      <c r="I37" s="13">
         <f t="shared" si="3"/>
         <v>3.2437624299403367E-3</v>
       </c>
-      <c r="J37" s="1">
+      <c r="J37" s="13">
         <f t="shared" si="4"/>
         <v>3.2898597231135968E-3</v>
       </c>
-      <c r="K37" s="1">
+      <c r="K37" s="13">
         <f t="shared" si="5"/>
         <v>3.4872910905435891E-3</v>
       </c>
@@ -6112,11 +6274,13 @@
       <c r="B38" s="1">
         <v>3.5539999999999998</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C38" s="13">
         <f t="shared" si="0"/>
         <v>3.5539999999999999E-3</v>
       </c>
-      <c r="D38" s="1"/>
+      <c r="D38" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E38" s="1">
         <v>1.1240000000000001</v>
       </c>
@@ -6128,16 +6292,18 @@
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1">
+      <c r="H38" s="1">
+        <v>32</v>
+      </c>
+      <c r="I38" s="13">
         <f t="shared" si="3"/>
         <v>3.3468871419535555E-3</v>
       </c>
-      <c r="J38" s="1">
+      <c r="J38" s="13">
         <f t="shared" si="4"/>
         <v>3.3959842303108094E-3</v>
       </c>
-      <c r="K38" s="1">
+      <c r="K38" s="13">
         <f t="shared" si="5"/>
         <v>3.593454781779035E-3</v>
       </c>
@@ -6153,11 +6319,13 @@
       <c r="B39" s="1">
         <v>3.64</v>
       </c>
-      <c r="C39" s="1">
+      <c r="C39" s="13">
         <f t="shared" si="0"/>
         <v>3.64E-3</v>
       </c>
-      <c r="D39" s="1"/>
+      <c r="D39" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E39" s="1">
         <v>1.125</v>
       </c>
@@ -6169,16 +6337,18 @@
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1">
+      <c r="H39" s="1">
+        <v>32</v>
+      </c>
+      <c r="I39" s="13">
         <f t="shared" si="3"/>
         <v>3.4499187138728321E-3</v>
       </c>
-      <c r="J39" s="1">
+      <c r="J39" s="13">
         <f t="shared" si="4"/>
         <v>3.5021087375080224E-3</v>
       </c>
-      <c r="K39" s="1">
+      <c r="K39" s="13">
         <f t="shared" si="5"/>
         <v>3.6996184730144809E-3</v>
       </c>
@@ -6194,11 +6364,13 @@
       <c r="B40" s="1">
         <v>3.7250000000000001</v>
       </c>
-      <c r="C40" s="1">
+      <c r="C40" s="13">
         <f t="shared" si="0"/>
         <v>3.725E-3</v>
       </c>
-      <c r="D40" s="1"/>
+      <c r="D40" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E40" s="1">
         <v>1.125</v>
       </c>
@@ -6210,16 +6382,18 @@
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1">
+      <c r="H40" s="1">
+        <v>32</v>
+      </c>
+      <c r="I40" s="13">
         <f t="shared" si="3"/>
         <v>3.4499187138728321E-3</v>
       </c>
-      <c r="J40" s="1">
+      <c r="J40" s="13">
         <f t="shared" si="4"/>
         <v>3.5021087375080224E-3</v>
       </c>
-      <c r="K40" s="1">
+      <c r="K40" s="13">
         <f t="shared" si="5"/>
         <v>3.6996184730144809E-3</v>
       </c>
@@ -6235,11 +6409,13 @@
       <c r="B41" s="1">
         <v>3.7930000000000001</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C41" s="13">
         <f t="shared" si="0"/>
         <v>3.7930000000000004E-3</v>
       </c>
-      <c r="D41" s="1"/>
+      <c r="D41" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E41" s="1">
         <v>1.1259999999999999</v>
       </c>
@@ -6251,16 +6427,18 @@
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1">
+      <c r="H41" s="1">
+        <v>32</v>
+      </c>
+      <c r="I41" s="13">
         <f t="shared" si="3"/>
         <v>3.5528572718245013E-3</v>
       </c>
-      <c r="J41" s="1">
+      <c r="J41" s="13">
         <f t="shared" si="4"/>
         <v>3.6082332447052354E-3</v>
       </c>
-      <c r="K41" s="1">
+      <c r="K41" s="13">
         <f t="shared" si="5"/>
         <v>3.8057821642499272E-3</v>
       </c>
@@ -6276,11 +6454,13 @@
       <c r="B42" s="1">
         <v>3.8479999999999999</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C42" s="13">
         <f t="shared" si="0"/>
         <v>3.8479999999999999E-3</v>
       </c>
-      <c r="D42" s="1"/>
+      <c r="D42" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E42" s="1">
         <v>1.127</v>
       </c>
@@ -6292,16 +6472,18 @@
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1">
+      <c r="H42" s="1">
+        <v>33</v>
+      </c>
+      <c r="I42" s="13">
         <f t="shared" si="3"/>
         <v>3.6557029417072732E-3</v>
       </c>
-      <c r="J42" s="1">
+      <c r="J42" s="13">
         <f t="shared" si="4"/>
         <v>3.7143577519024485E-3</v>
       </c>
-      <c r="K42" s="1">
+      <c r="K42" s="13">
         <f t="shared" si="5"/>
         <v>3.9119458554853735E-3</v>
       </c>
@@ -6317,11 +6499,13 @@
       <c r="B43" s="1">
         <v>3.9119999999999999</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43" s="13">
         <f t="shared" si="0"/>
         <v>3.9119999999999997E-3</v>
       </c>
-      <c r="D43" s="1"/>
+      <c r="D43" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E43" s="1">
         <v>1.127</v>
       </c>
@@ -6333,16 +6517,18 @@
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1">
+      <c r="H43" s="1">
+        <v>33</v>
+      </c>
+      <c r="I43" s="13">
         <f t="shared" si="3"/>
         <v>3.6557029417072732E-3</v>
       </c>
-      <c r="J43" s="1">
+      <c r="J43" s="13">
         <f t="shared" si="4"/>
         <v>3.7143577519024485E-3</v>
       </c>
-      <c r="K43" s="1">
+      <c r="K43" s="13">
         <f t="shared" si="5"/>
         <v>3.9119458554853735E-3</v>
       </c>
@@ -6358,11 +6544,13 @@
       <c r="B44" s="1">
         <v>3.9790000000000001</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44" s="13">
         <f t="shared" si="0"/>
         <v>3.9789999999999999E-3</v>
       </c>
-      <c r="D44" s="1"/>
+      <c r="D44" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E44" s="1">
         <v>1.127</v>
       </c>
@@ -6374,16 +6562,18 @@
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1">
+      <c r="H44" s="1">
+        <v>33</v>
+      </c>
+      <c r="I44" s="13">
         <f t="shared" si="3"/>
         <v>3.6557029417072732E-3</v>
       </c>
-      <c r="J44" s="1">
+      <c r="J44" s="13">
         <f t="shared" si="4"/>
         <v>3.7143577519024485E-3</v>
       </c>
-      <c r="K44" s="1">
+      <c r="K44" s="13">
         <f t="shared" si="5"/>
         <v>3.9119458554853735E-3</v>
       </c>
@@ -6399,11 +6589,13 @@
       <c r="B45" s="1">
         <v>4.0419999999999998</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45" s="13">
         <f t="shared" si="0"/>
         <v>4.0419999999999996E-3</v>
       </c>
-      <c r="D45" s="1"/>
+      <c r="D45" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E45" s="1">
         <v>1.1279999999999999</v>
       </c>
@@ -6415,16 +6607,18 @@
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1">
+      <c r="H45" s="1">
+        <v>33</v>
+      </c>
+      <c r="I45" s="13">
         <f t="shared" si="3"/>
         <v>3.7584558491927478E-3</v>
       </c>
-      <c r="J45" s="1">
+      <c r="J45" s="13">
         <f t="shared" si="4"/>
         <v>3.8204822590996606E-3</v>
       </c>
-      <c r="K45" s="1">
+      <c r="K45" s="13">
         <f t="shared" si="5"/>
         <v>4.0181095467208194E-3</v>
       </c>
@@ -6440,11 +6634,13 @@
       <c r="B46" s="1">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C46" s="13">
         <f t="shared" si="0"/>
         <v>4.0999999999999995E-3</v>
       </c>
-      <c r="D46" s="1"/>
+      <c r="D46" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E46" s="1">
         <v>1.129</v>
       </c>
@@ -6456,16 +6652,18 @@
         <f t="shared" si="2"/>
         <v>37</v>
       </c>
-      <c r="H46" s="1"/>
-      <c r="I46" s="1">
+      <c r="H46" s="1">
+        <v>33</v>
+      </c>
+      <c r="I46" s="13">
         <f t="shared" si="3"/>
         <v>3.8611161197259283E-3</v>
       </c>
-      <c r="J46" s="1">
+      <c r="J46" s="13">
         <f t="shared" si="4"/>
         <v>3.9266067662968732E-3</v>
       </c>
-      <c r="K46" s="1">
+      <c r="K46" s="13">
         <f t="shared" si="5"/>
         <v>4.1242732379562653E-3</v>
       </c>
@@ -6481,11 +6679,13 @@
       <c r="B47" s="1">
         <v>4.16</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C47" s="13">
         <f t="shared" si="0"/>
         <v>4.1600000000000005E-3</v>
       </c>
-      <c r="D47" s="1"/>
+      <c r="D47" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E47" s="1">
         <v>1.1299999999999999</v>
       </c>
@@ -6497,16 +6697,18 @@
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1">
+      <c r="H47" s="1">
+        <v>33</v>
+      </c>
+      <c r="I47" s="13">
         <f t="shared" si="3"/>
         <v>3.9636838785257278E-3</v>
       </c>
-      <c r="J47" s="1">
+      <c r="J47" s="13">
         <f t="shared" si="4"/>
         <v>4.0327312734940862E-3</v>
       </c>
-      <c r="K47" s="1">
+      <c r="K47" s="13">
         <f t="shared" si="5"/>
         <v>4.2304369291917112E-3</v>
       </c>
@@ -6522,11 +6724,13 @@
       <c r="B48" s="1">
         <v>4.2140000000000004</v>
       </c>
-      <c r="C48" s="1">
+      <c r="C48" s="13">
         <f t="shared" si="0"/>
         <v>4.2140000000000007E-3</v>
       </c>
-      <c r="D48" s="1"/>
+      <c r="D48" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E48" s="1">
         <v>1.1299999999999999</v>
       </c>
@@ -6538,16 +6742,18 @@
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="H48" s="1"/>
-      <c r="I48" s="1">
+      <c r="H48" s="1">
+        <v>33</v>
+      </c>
+      <c r="I48" s="13">
         <f t="shared" si="3"/>
         <v>3.9636838785257278E-3</v>
       </c>
-      <c r="J48" s="1">
+      <c r="J48" s="13">
         <f t="shared" si="4"/>
         <v>4.0327312734940862E-3</v>
       </c>
-      <c r="K48" s="1">
+      <c r="K48" s="13">
         <f t="shared" si="5"/>
         <v>4.2304369291917112E-3</v>
       </c>
@@ -6563,11 +6769,13 @@
       <c r="B49" s="1">
         <v>4.266</v>
       </c>
-      <c r="C49" s="1">
+      <c r="C49" s="13">
         <f t="shared" si="0"/>
         <v>4.2659999999999998E-3</v>
       </c>
-      <c r="D49" s="1"/>
+      <c r="D49" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E49" s="1">
         <v>1.1299999999999999</v>
       </c>
@@ -6579,16 +6787,18 @@
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1">
+      <c r="H49" s="1">
+        <v>33</v>
+      </c>
+      <c r="I49" s="13">
         <f t="shared" si="3"/>
         <v>3.9636838785257278E-3</v>
       </c>
-      <c r="J49" s="1">
+      <c r="J49" s="13">
         <f t="shared" si="4"/>
         <v>4.0327312734940862E-3</v>
       </c>
-      <c r="K49" s="1">
+      <c r="K49" s="13">
         <f t="shared" si="5"/>
         <v>4.2304369291917112E-3</v>
       </c>
@@ -6604,11 +6814,13 @@
       <c r="B50" s="1">
         <v>4.3129999999999997</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C50" s="13">
         <f t="shared" si="0"/>
         <v>4.313E-3</v>
       </c>
-      <c r="D50" s="1"/>
+      <c r="D50" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E50" s="1">
         <v>1.131</v>
       </c>
@@ -6620,16 +6832,18 @@
         <f t="shared" si="2"/>
         <v>39</v>
       </c>
-      <c r="H50" s="1"/>
-      <c r="I50" s="1">
+      <c r="H50" s="1">
+        <v>34</v>
+      </c>
+      <c r="I50" s="13">
         <f t="shared" si="3"/>
         <v>4.0661592505854801E-3</v>
       </c>
-      <c r="J50" s="1">
+      <c r="J50" s="13">
         <f t="shared" si="4"/>
         <v>4.1388557806912992E-3</v>
       </c>
-      <c r="K50" s="1">
+      <c r="K50" s="13">
         <f t="shared" si="5"/>
         <v>4.336600620427157E-3</v>
       </c>
@@ -6645,11 +6859,13 @@
       <c r="B51" s="1">
         <v>4.3780000000000001</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C51" s="13">
         <f t="shared" si="0"/>
         <v>4.3779999999999999E-3</v>
       </c>
-      <c r="D51" s="1"/>
+      <c r="D51" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E51" s="1">
         <v>1.131</v>
       </c>
@@ -6661,16 +6877,18 @@
         <f t="shared" si="2"/>
         <v>39</v>
       </c>
-      <c r="H51" s="1"/>
-      <c r="I51" s="1">
+      <c r="H51" s="1">
+        <v>34</v>
+      </c>
+      <c r="I51" s="13">
         <f t="shared" si="3"/>
         <v>4.0661592505854801E-3</v>
       </c>
-      <c r="J51" s="1">
+      <c r="J51" s="13">
         <f t="shared" si="4"/>
         <v>4.1388557806912992E-3</v>
       </c>
-      <c r="K51" s="1">
+      <c r="K51" s="13">
         <f t="shared" si="5"/>
         <v>4.336600620427157E-3</v>
       </c>
@@ -6686,11 +6904,13 @@
       <c r="B52" s="1">
         <v>4.4260000000000002</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C52" s="13">
         <f t="shared" si="0"/>
         <v>4.4260000000000002E-3</v>
       </c>
-      <c r="D52" s="1"/>
+      <c r="D52" s="13">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E52" s="1">
         <v>1.1319999999999999</v>
       </c>
@@ -6702,16 +6922,18 @@
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="H52" s="1"/>
-      <c r="I52" s="1">
+      <c r="H52" s="1">
+        <v>34</v>
+      </c>
+      <c r="I52" s="13">
         <f t="shared" si="3"/>
         <v>4.1685423606734485E-3</v>
       </c>
-      <c r="J52" s="1">
+      <c r="J52" s="13">
         <f t="shared" si="4"/>
         <v>4.2449802878885114E-3</v>
       </c>
-      <c r="K52" s="1">
+      <c r="K52" s="13">
         <f t="shared" si="5"/>
         <v>4.4427643116626038E-3</v>
       </c>

</xml_diff>